<commit_message>
Fixed some loose ends when using AMID analysis
Also cleaned up some units in graphs
</commit_message>
<xml_diff>
--- a/Analyzed Data/NM9505 30C Old/215 NM9505 30C Old Charge Filtered.xlsx
+++ b/Analyzed Data/NM9505 30C Old/215 NM9505 30C Old Charge Filtered.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,848 +502,821 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3.579412188613863</v>
+        <v>3.620736049009901</v>
       </c>
       <c r="B2" t="n">
-        <v>3.556449612871288</v>
+        <v>3.602374764356437</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9304681353507841</v>
+        <v>0.8867182122118554</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9543142967306345</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+        <v>0.9066219977820681</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.674339979820928e-13</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.354412011025889e-13</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.181869159703924</v>
+      </c>
       <c r="H2" t="n">
-        <v>292.7595327000748</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+        <v>306.3927289448299</v>
+      </c>
+      <c r="I2" t="n">
+        <v>10195.63210908549</v>
+      </c>
+      <c r="J2" t="n">
+        <v>28464.1613649022</v>
+      </c>
       <c r="K2" t="n">
-        <v>296.2240691933535</v>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+        <v>293.2885201074942</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.7659174979710912</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0392131388442514</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.620736049009901</v>
+        <v>3.652924425247525</v>
       </c>
       <c r="B3" t="n">
-        <v>3.602374764356437</v>
+        <v>3.639097333663365</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8867182122118554</v>
+        <v>0.8391446026191456</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9066219977820681</v>
+        <v>0.8668144507331865</v>
       </c>
       <c r="E3" t="n">
-        <v>4.674339979820928e-13</v>
+        <v>4.777788983538347e-13</v>
       </c>
       <c r="F3" t="n">
-        <v>1.354412011025889e-13</v>
+        <v>1.899434767816931e-13</v>
       </c>
       <c r="G3" t="n">
-        <v>0.181869159703924</v>
+        <v>0.1545666664453009</v>
       </c>
       <c r="H3" t="n">
-        <v>306.3927289448299</v>
+        <v>564.9006757097389</v>
       </c>
       <c r="I3" t="n">
-        <v>10195.63210908549</v>
+        <v>4598.01760050979</v>
       </c>
       <c r="J3" t="n">
-        <v>28464.1613649022</v>
+        <v>12836.74357207759</v>
       </c>
       <c r="K3" t="n">
-        <v>293.2885201074942</v>
+        <v>303.2142964760513</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7659174979710912</v>
+        <v>0.7909115700907602</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0392131388442514</v>
+        <v>0.01817640339941046</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.652924425247525</v>
+        <v>3.679524980693071</v>
       </c>
       <c r="B4" t="n">
-        <v>3.639097333663365</v>
+        <v>3.666751516831685</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8391446026191456</v>
+        <v>0.7928317718033387</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8668144507331865</v>
+        <v>0.8114747781125126</v>
       </c>
       <c r="E4" t="n">
-        <v>4.777788983538347e-13</v>
+        <v>9.517234291239773e-13</v>
       </c>
       <c r="F4" t="n">
-        <v>1.899434767816931e-13</v>
+        <v>2.275811002987144e-13</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1545666664453009</v>
+        <v>0.1179421707963817</v>
       </c>
       <c r="H4" t="n">
-        <v>564.9006757097389</v>
+        <v>413.4584401332804</v>
       </c>
       <c r="I4" t="n">
-        <v>4598.01760050979</v>
+        <v>2406.469391607144</v>
       </c>
       <c r="J4" t="n">
-        <v>12836.74357207759</v>
+        <v>6718.380219051252</v>
       </c>
       <c r="K4" t="n">
-        <v>303.2142964760513</v>
+        <v>309.7293391047671</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7909115700907602</v>
+        <v>0.7914483437961572</v>
       </c>
       <c r="M4" t="n">
-        <v>0.01817640339941046</v>
+        <v>0.03733316685678481</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.679524980693071</v>
+        <v>3.699255869801981</v>
       </c>
       <c r="B5" t="n">
-        <v>3.666751516831685</v>
+        <v>3.686422283168319</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7928317718033387</v>
+        <v>0.7607776126703595</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8114747781125126</v>
+        <v>0.7741888599260756</v>
       </c>
       <c r="E5" t="n">
-        <v>9.517234291239773e-13</v>
+        <v>2.452535929260104e-12</v>
       </c>
       <c r="F5" t="n">
-        <v>2.275811002987144e-13</v>
+        <v>3.745620174033873e-13</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1179421707963817</v>
+        <v>0.1764132971234397</v>
       </c>
       <c r="H5" t="n">
-        <v>413.4584401332804</v>
+        <v>292.5971783174842</v>
       </c>
       <c r="I5" t="n">
-        <v>2406.469391607144</v>
+        <v>1973.784129073736</v>
       </c>
       <c r="J5" t="n">
-        <v>6718.380219051252</v>
+        <v>5510.409688024441</v>
       </c>
       <c r="K5" t="n">
-        <v>309.7293391047671</v>
+        <v>297.2404848456374</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7914483437961572</v>
+        <v>0.6593096409208157</v>
       </c>
       <c r="M5" t="n">
-        <v>0.03733316685678481</v>
+        <v>0.01061917125758657</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.699255869801981</v>
+        <v>3.725343482673266</v>
       </c>
       <c r="B6" t="n">
-        <v>3.686422283168319</v>
+        <v>3.712089456435642</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7607776126703595</v>
+        <v>0.7326739465384652</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7741888599260756</v>
+        <v>0.7473663881730492</v>
       </c>
       <c r="E6" t="n">
-        <v>2.452535929260104e-12</v>
+        <v>2.072442625261879e-12</v>
       </c>
       <c r="F6" t="n">
-        <v>3.745620174033873e-13</v>
+        <v>3.139433694767128e-13</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1764132971234397</v>
+        <v>0.1038111066763614</v>
       </c>
       <c r="H6" t="n">
-        <v>292.5971783174842</v>
+        <v>312.3367355172376</v>
       </c>
       <c r="I6" t="n">
-        <v>1973.784129073736</v>
+        <v>1287.632962103033</v>
       </c>
       <c r="J6" t="n">
-        <v>5510.409688024441</v>
+        <v>3594.81315331171</v>
       </c>
       <c r="K6" t="n">
-        <v>297.2404848456374</v>
+        <v>277.2184836638315</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6593096409208157</v>
+        <v>0.7342393905561173</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01061917125758657</v>
+        <v>0.01767276991469401</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.725343482673266</v>
+        <v>3.751519974752475</v>
       </c>
       <c r="B7" t="n">
-        <v>3.712089456435642</v>
+        <v>3.73859750891089</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7326739465384652</v>
+        <v>0.7025972164436267</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7473663881730492</v>
+        <v>0.717981527635466</v>
       </c>
       <c r="E7" t="n">
-        <v>2.072442625261879e-12</v>
+        <v>1.926300540431125e-12</v>
       </c>
       <c r="F7" t="n">
-        <v>3.139433694767128e-13</v>
+        <v>2.943717855679378e-13</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1038111066763614</v>
+        <v>0.07283612231744398</v>
       </c>
       <c r="H7" t="n">
-        <v>312.3367355172376</v>
+        <v>336.1443546075569</v>
       </c>
       <c r="I7" t="n">
-        <v>1287.632962103033</v>
+        <v>903.1310962002477</v>
       </c>
       <c r="J7" t="n">
-        <v>3594.81315331171</v>
+        <v>2521.361008406439</v>
       </c>
       <c r="K7" t="n">
-        <v>277.2184836638315</v>
+        <v>262.0603374883909</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7342393905561173</v>
+        <v>0.7453934569208772</v>
       </c>
       <c r="M7" t="n">
-        <v>0.01767276991469401</v>
+        <v>0.02122636044020544</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.751519974752475</v>
+        <v>3.776996204950495</v>
       </c>
       <c r="B8" t="n">
-        <v>3.73859750891089</v>
+        <v>3.764442440594061</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7025972164436267</v>
+        <v>0.6721163486365607</v>
       </c>
       <c r="D8" t="n">
-        <v>0.717981527635466</v>
+        <v>0.6872129288068618</v>
       </c>
       <c r="E8" t="n">
-        <v>1.926300540431125e-12</v>
+        <v>2.177590428350819e-12</v>
       </c>
       <c r="F8" t="n">
-        <v>2.943717855679378e-13</v>
+        <v>3.187850862341234e-13</v>
       </c>
       <c r="G8" t="n">
-        <v>0.07283612231744398</v>
+        <v>0.06470195287340186</v>
       </c>
       <c r="H8" t="n">
-        <v>336.1443546075569</v>
+        <v>339.6160848993548</v>
       </c>
       <c r="I8" t="n">
-        <v>903.1310962002477</v>
+        <v>702.4360413492959</v>
       </c>
       <c r="J8" t="n">
-        <v>2521.361008406439</v>
+        <v>1961.060640043325</v>
       </c>
       <c r="K8" t="n">
-        <v>262.0603374883909</v>
+        <v>249.846899710702</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7453934569208772</v>
+        <v>0.7577692386094314</v>
       </c>
       <c r="M8" t="n">
-        <v>0.02122636044020544</v>
+        <v>0.02558827496655998</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.776996204950495</v>
+        <v>3.801840694554455</v>
       </c>
       <c r="B9" t="n">
-        <v>3.764442440594061</v>
+        <v>3.789549969306929</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6721163486365607</v>
+        <v>0.6437276347212123</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6872129288068618</v>
+        <v>0.6570197922644265</v>
       </c>
       <c r="E9" t="n">
-        <v>2.177590428350819e-12</v>
+        <v>2.743884507089316e-12</v>
       </c>
       <c r="F9" t="n">
-        <v>3.187850862341234e-13</v>
+        <v>3.475441159866836e-13</v>
       </c>
       <c r="G9" t="n">
-        <v>0.06470195287340186</v>
+        <v>0.06254332854026885</v>
       </c>
       <c r="H9" t="n">
-        <v>339.6160848993548</v>
+        <v>305.7951798484341</v>
       </c>
       <c r="I9" t="n">
-        <v>702.4360413492959</v>
+        <v>598.464474486436</v>
       </c>
       <c r="J9" t="n">
-        <v>1961.060640043325</v>
+        <v>1670.792864109263</v>
       </c>
       <c r="K9" t="n">
-        <v>249.846899710702</v>
+        <v>242.2979038551237</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7577692386094314</v>
+        <v>0.7395780100269461</v>
       </c>
       <c r="M9" t="n">
-        <v>0.02558827496655998</v>
+        <v>0.03082776332027542</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.801840694554455</v>
+        <v>3.826308996039604</v>
       </c>
       <c r="B10" t="n">
-        <v>3.789549969306929</v>
+        <v>3.814131419801981</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6437276347212123</v>
+        <v>0.6193606523952206</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6570197922644265</v>
+        <v>0.6304355006729732</v>
       </c>
       <c r="E10" t="n">
-        <v>2.743884507089316e-12</v>
+        <v>3.091543489219953e-12</v>
       </c>
       <c r="F10" t="n">
-        <v>3.475441159866836e-13</v>
+        <v>3.202706894299775e-13</v>
       </c>
       <c r="G10" t="n">
-        <v>0.06254332854026885</v>
+        <v>0.05180083386036843</v>
       </c>
       <c r="H10" t="n">
-        <v>305.7951798484341</v>
+        <v>257.0995749171279</v>
       </c>
       <c r="I10" t="n">
-        <v>598.464474486436</v>
+        <v>523.2555938116038</v>
       </c>
       <c r="J10" t="n">
-        <v>1670.792864109263</v>
+        <v>1460.824743182809</v>
       </c>
       <c r="K10" t="n">
-        <v>242.2979038551237</v>
+        <v>224.7658402459299</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7395780100269461</v>
+        <v>0.7385240711062502</v>
       </c>
       <c r="M10" t="n">
-        <v>0.03082776332027542</v>
+        <v>0.04277761590095808</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3.826308996039604</v>
+        <v>3.850743871782178</v>
       </c>
       <c r="B11" t="n">
-        <v>3.814131419801981</v>
+        <v>3.838486572277227</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6193606523952206</v>
+        <v>0.5988632757310339</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6304355006729732</v>
+        <v>0.6082858277787302</v>
       </c>
       <c r="E11" t="n">
-        <v>3.091543489219953e-12</v>
+        <v>3.294781467506547e-12</v>
       </c>
       <c r="F11" t="n">
-        <v>3.202706894299775e-13</v>
+        <v>2.835522585371362e-13</v>
       </c>
       <c r="G11" t="n">
-        <v>0.05180083386036843</v>
+        <v>0.04368793331503201</v>
       </c>
       <c r="H11" t="n">
-        <v>257.0995749171279</v>
+        <v>217.6350471697538</v>
       </c>
       <c r="I11" t="n">
-        <v>523.2555938116038</v>
+        <v>489.1700961640038</v>
       </c>
       <c r="J11" t="n">
-        <v>1460.824743182809</v>
+        <v>1365.664865417142</v>
       </c>
       <c r="K11" t="n">
-        <v>224.7658402459299</v>
+        <v>226.6664782412236</v>
       </c>
       <c r="L11" t="n">
-        <v>0.7385240711062502</v>
+        <v>0.7089262025549914</v>
       </c>
       <c r="M11" t="n">
-        <v>0.04277761590095808</v>
+        <v>0.04780999974932559</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3.850743871782178</v>
+        <v>3.875415429207921</v>
       </c>
       <c r="B12" t="n">
-        <v>3.838486572277227</v>
+        <v>3.863001171287128</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5988632757310339</v>
+        <v>0.5807429553881358</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6082858277787302</v>
+        <v>0.5894407477746866</v>
       </c>
       <c r="E12" t="n">
-        <v>3.294781467506547e-12</v>
+        <v>3.195398351896032e-12</v>
       </c>
       <c r="F12" t="n">
-        <v>2.835522585371362e-13</v>
+        <v>2.466320605509448e-13</v>
       </c>
       <c r="G12" t="n">
-        <v>0.04368793331503201</v>
+        <v>0.03659573319560247</v>
       </c>
       <c r="H12" t="n">
-        <v>217.6350471697538</v>
+        <v>197.8295102290545</v>
       </c>
       <c r="I12" t="n">
-        <v>489.1700961640038</v>
+        <v>464.8022457713583</v>
       </c>
       <c r="J12" t="n">
-        <v>1365.664865417142</v>
+        <v>1297.634711104888</v>
       </c>
       <c r="K12" t="n">
-        <v>226.6664782412236</v>
+        <v>216.3212351864397</v>
       </c>
       <c r="L12" t="n">
-        <v>0.7089262025549914</v>
+        <v>0.7099479229005424</v>
       </c>
       <c r="M12" t="n">
-        <v>0.04780999974932559</v>
+        <v>0.05451936166650542</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3.875415429207921</v>
+        <v>3.90044154108911</v>
       </c>
       <c r="B13" t="n">
-        <v>3.863001171287128</v>
+        <v>3.887829687128713</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5807429553881358</v>
+        <v>0.5631387433020947</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5894407477746866</v>
+        <v>0.5720451860200731</v>
       </c>
       <c r="E13" t="n">
-        <v>3.195398351896032e-12</v>
+        <v>2.833703830251788e-12</v>
       </c>
       <c r="F13" t="n">
-        <v>2.466320605509448e-13</v>
+        <v>2.180664924659718e-13</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03659573319560247</v>
+        <v>0.03252370066464468</v>
       </c>
       <c r="H13" t="n">
-        <v>197.8295102290545</v>
+        <v>199.2946550359908</v>
       </c>
       <c r="I13" t="n">
-        <v>464.8022457713583</v>
+        <v>462.3849548924079</v>
       </c>
       <c r="J13" t="n">
-        <v>1297.634711104888</v>
+        <v>1290.886119462097</v>
       </c>
       <c r="K13" t="n">
-        <v>216.3212351864397</v>
+        <v>218.1305466599291</v>
       </c>
       <c r="L13" t="n">
-        <v>0.7099479229005424</v>
+        <v>0.7079474592346549</v>
       </c>
       <c r="M13" t="n">
-        <v>0.05451936166650542</v>
+        <v>0.05512511671293405</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.90044154108911</v>
+        <v>3.925914226732674</v>
       </c>
       <c r="B14" t="n">
-        <v>3.887829687128713</v>
+        <v>3.913053395049507</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5631387433020947</v>
+        <v>0.5438958214577525</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5720451860200731</v>
+        <v>0.5542323237481271</v>
       </c>
       <c r="E14" t="n">
-        <v>2.833703830251788e-12</v>
+        <v>2.305133281366189e-12</v>
       </c>
       <c r="F14" t="n">
-        <v>2.180664924659718e-13</v>
+        <v>2.004109941404972e-13</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03252370066464468</v>
+        <v>0.0300453597952817</v>
       </c>
       <c r="H14" t="n">
-        <v>199.2946550359908</v>
+        <v>227.0426812356649</v>
       </c>
       <c r="I14" t="n">
-        <v>462.3849548924079</v>
+        <v>460.9222877986647</v>
       </c>
       <c r="J14" t="n">
-        <v>1290.886119462097</v>
+        <v>1286.802646094875</v>
       </c>
       <c r="K14" t="n">
-        <v>218.1305466599291</v>
+        <v>218.1482194702695</v>
       </c>
       <c r="L14" t="n">
-        <v>0.7079474592346549</v>
+        <v>0.6898245021048733</v>
       </c>
       <c r="M14" t="n">
-        <v>0.05512511671293405</v>
+        <v>0.05181221135086551</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.925914226732674</v>
+        <v>3.950714869801978</v>
       </c>
       <c r="B15" t="n">
-        <v>3.913053395049507</v>
+        <v>3.938775058415841</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5438958214577525</v>
+        <v>0.5206794560569086</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5542323237481271</v>
+        <v>0.5335593429547203</v>
       </c>
       <c r="E15" t="n">
-        <v>2.305133281366189e-12</v>
+        <v>1.485216187529089e-12</v>
       </c>
       <c r="F15" t="n">
-        <v>2.004109941404972e-13</v>
+        <v>1.730335697204537e-13</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0300453597952817</v>
+        <v>0.02557460960990082</v>
       </c>
       <c r="H15" t="n">
-        <v>227.0426812356649</v>
+        <v>306.0831426554146</v>
       </c>
       <c r="I15" t="n">
-        <v>460.9222877986647</v>
+        <v>451.6830309006478</v>
       </c>
       <c r="J15" t="n">
-        <v>1286.802646094875</v>
+        <v>1261.008492635514</v>
       </c>
       <c r="K15" t="n">
-        <v>218.1482194702695</v>
+        <v>209.8397274580574</v>
       </c>
       <c r="L15" t="n">
-        <v>0.6898245021048733</v>
+        <v>0.670927046716905</v>
       </c>
       <c r="M15" t="n">
-        <v>0.05181221135086551</v>
+        <v>0.05522688189610096</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.950714869801978</v>
+        <v>3.988036308415839</v>
       </c>
       <c r="B16" t="n">
-        <v>3.938775058415841</v>
+        <v>3.962654681188115</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5206794560569086</v>
+        <v>0.4740770199242028</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5335593429547203</v>
+        <v>0.5077995931320249</v>
       </c>
       <c r="E16" t="n">
-        <v>1.485216187529089e-12</v>
+        <v>1.198825112716417e-12</v>
       </c>
       <c r="F16" t="n">
-        <v>1.730335697204537e-13</v>
+        <v>1.703961310839761e-13</v>
       </c>
       <c r="G16" t="n">
-        <v>0.02557460960990082</v>
+        <v>0.02574372683017588</v>
       </c>
       <c r="H16" t="n">
-        <v>306.0831426554146</v>
+        <v>373.0587080785905</v>
       </c>
       <c r="I16" t="n">
-        <v>451.6830309006478</v>
+        <v>462.1598913041465</v>
       </c>
       <c r="J16" t="n">
-        <v>1261.008492635514</v>
+        <v>1290.257787032572</v>
       </c>
       <c r="K16" t="n">
-        <v>209.8397274580574</v>
+        <v>217.932138656296</v>
       </c>
       <c r="L16" t="n">
-        <v>0.670927046716905</v>
+        <v>0.8583306780958588</v>
       </c>
       <c r="M16" t="n">
-        <v>0.05522688189610096</v>
+        <v>0.04578531047645357</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.988036308415839</v>
+        <v>4.024957870792079</v>
       </c>
       <c r="B17" t="n">
-        <v>3.962654681188115</v>
+        <v>4.013417935643562</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4740770199242028</v>
+        <v>0.4269027628961122</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5077995931320249</v>
+        <v>0.4403544670642062</v>
       </c>
       <c r="E17" t="n">
-        <v>1.198825112716417e-12</v>
+        <v>2.20637223310912e-12</v>
       </c>
       <c r="F17" t="n">
-        <v>1.703961310839761e-13</v>
+        <v>2.825040073664013e-13</v>
       </c>
       <c r="G17" t="n">
-        <v>0.02574372683017588</v>
+        <v>0.04253045249783072</v>
       </c>
       <c r="H17" t="n">
-        <v>373.0587080785905</v>
+        <v>329.7655942476229</v>
       </c>
       <c r="I17" t="n">
-        <v>462.1598913041465</v>
+        <v>469.3207173079945</v>
       </c>
       <c r="J17" t="n">
-        <v>1290.257787032572</v>
+        <v>1310.249378009838</v>
       </c>
       <c r="K17" t="n">
-        <v>217.932138656296</v>
+        <v>203.4688109502742</v>
       </c>
       <c r="L17" t="n">
-        <v>0.8583306780958588</v>
+        <v>0.6840435647058986</v>
       </c>
       <c r="M17" t="n">
-        <v>0.04578531047645357</v>
+        <v>0.0490343386774681</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.024957870792079</v>
+        <v>4.048143822277227</v>
       </c>
       <c r="B18" t="n">
-        <v>4.013417935643562</v>
+        <v>4.036497805940595</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4269027628961122</v>
+        <v>0.4034390973046975</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4403544670642062</v>
+        <v>0.4134510778556927</v>
       </c>
       <c r="E18" t="n">
-        <v>2.20637223310912e-12</v>
+        <v>2.477912784573757e-12</v>
       </c>
       <c r="F18" t="n">
-        <v>2.825040073664013e-13</v>
+        <v>2.380278948604979e-13</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04253045249783072</v>
+        <v>0.03421050198238342</v>
       </c>
       <c r="H18" t="n">
-        <v>329.7655942476229</v>
+        <v>243.3754918826698</v>
       </c>
       <c r="I18" t="n">
-        <v>469.3207173079945</v>
+        <v>455.4602035135529</v>
       </c>
       <c r="J18" t="n">
-        <v>1310.249378009838</v>
+        <v>1271.553601521997</v>
       </c>
       <c r="K18" t="n">
-        <v>203.4688109502742</v>
+        <v>210.5903088285731</v>
       </c>
       <c r="L18" t="n">
-        <v>0.6840435647058986</v>
+        <v>0.6408846283911489</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0490343386774681</v>
+        <v>0.06437935650533816</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4.048143822277227</v>
+        <v>4.071631842079206</v>
       </c>
       <c r="B19" t="n">
-        <v>4.036497805940595</v>
+        <v>4.059789838613859</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4034390973046975</v>
+        <v>0.3854256130262844</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4134510778556927</v>
+        <v>0.3934271355826724</v>
       </c>
       <c r="E19" t="n">
-        <v>2.477912784573757e-12</v>
+        <v>2.632443897963255e-12</v>
       </c>
       <c r="F19" t="n">
-        <v>2.380278948604979e-13</v>
+        <v>2.020451493985933e-13</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03421050198238342</v>
+        <v>0.02757365956371339</v>
       </c>
       <c r="H19" t="n">
-        <v>243.3754918826698</v>
+        <v>191.3844132272695</v>
       </c>
       <c r="I19" t="n">
-        <v>455.4602035135529</v>
+        <v>439.4227803929551</v>
       </c>
       <c r="J19" t="n">
-        <v>1271.553601521997</v>
+        <v>1226.780330507723</v>
       </c>
       <c r="K19" t="n">
-        <v>210.5903088285731</v>
+        <v>201.9585081673409</v>
       </c>
       <c r="L19" t="n">
-        <v>0.6408846283911489</v>
+        <v>0.5868970326900731</v>
       </c>
       <c r="M19" t="n">
-        <v>0.06437935650533816</v>
+        <v>0.07663980245787663</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>4.071631842079206</v>
+        <v>4.095792353465347</v>
       </c>
       <c r="B20" t="n">
-        <v>4.059789838613859</v>
+        <v>4.083473845544553</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3854256130262844</v>
+        <v>0.37037748200145</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3934271355826724</v>
+        <v>0.3774241090637914</v>
       </c>
       <c r="E20" t="n">
-        <v>2.632443897963255e-12</v>
+        <v>2.524362095987949e-12</v>
       </c>
       <c r="F20" t="n">
-        <v>2.020451493985933e-13</v>
+        <v>1.663348517596428e-13</v>
       </c>
       <c r="G20" t="n">
-        <v>0.02757365956371339</v>
+        <v>0.02200772624111243</v>
       </c>
       <c r="H20" t="n">
-        <v>191.3844132272695</v>
+        <v>161.755353825679</v>
       </c>
       <c r="I20" t="n">
-        <v>439.4227803929551</v>
+        <v>432.7316975595347</v>
       </c>
       <c r="J20" t="n">
-        <v>1226.780330507723</v>
+        <v>1208.100168312906</v>
       </c>
       <c r="K20" t="n">
-        <v>201.9585081673409</v>
+        <v>205.5170880846259</v>
       </c>
       <c r="L20" t="n">
-        <v>0.5868970326900731</v>
+        <v>0.5853192699162105</v>
       </c>
       <c r="M20" t="n">
-        <v>0.07663980245787663</v>
+        <v>0.08457691017045862</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>4.095792353465347</v>
+        <v>4.121131645544557</v>
       </c>
       <c r="B21" t="n">
-        <v>4.083473845544553</v>
+        <v>4.10811086138614</v>
       </c>
       <c r="C21" t="n">
-        <v>0.37037748200145</v>
+        <v>0.3562569693507968</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3774241090637914</v>
+        <v>0.3633308736154864</v>
       </c>
       <c r="E21" t="n">
-        <v>2.524362095987949e-12</v>
+        <v>2.398903864701567e-12</v>
       </c>
       <c r="F21" t="n">
-        <v>1.663348517596428e-13</v>
+        <v>1.525841309939344e-13</v>
       </c>
       <c r="G21" t="n">
-        <v>0.02200772624111243</v>
+        <v>0.0208516692420542</v>
       </c>
       <c r="H21" t="n">
-        <v>161.755353825679</v>
+        <v>153.5587846369461</v>
       </c>
       <c r="I21" t="n">
-        <v>432.7316975595347</v>
+        <v>454.4720348444612</v>
       </c>
       <c r="J21" t="n">
-        <v>1208.100168312906</v>
+        <v>1268.794832653934</v>
       </c>
       <c r="K21" t="n">
-        <v>205.5170880846259</v>
+        <v>212.9394839655679</v>
       </c>
       <c r="L21" t="n">
-        <v>0.5853192699162105</v>
+        <v>0.5914270842581743</v>
       </c>
       <c r="M21" t="n">
-        <v>0.08457691017045862</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>4.121131645544557</v>
-      </c>
-      <c r="B22" t="n">
-        <v>4.10811086138614</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.3562569693507968</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.3633308736154864</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2.398903864701567e-12</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1.525841309939344e-13</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.0208516692420542</v>
-      </c>
-      <c r="H22" t="n">
-        <v>153.5587846369461</v>
-      </c>
-      <c r="I22" t="n">
-        <v>454.4720348444612</v>
-      </c>
-      <c r="J22" t="n">
-        <v>1268.794832653934</v>
-      </c>
-      <c r="K22" t="n">
-        <v>212.9394839655679</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.5914270842581743</v>
-      </c>
-      <c r="M22" t="n">
         <v>0.08174543104801593</v>
       </c>
     </row>

</xml_diff>